<commit_message>
Wszystko nie działa, jestem głupi
</commit_message>
<xml_diff>
--- a/wb.xlsx
+++ b/wb.xlsx
@@ -180,7 +180,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -234,9 +234,6 @@
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="G2" s="0" t="n">
         <v>6951</v>
       </c>
@@ -266,9 +263,6 @@
       <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <v>2</v>
-      </c>
       <c r="G3" s="0" t="n">
         <v>7023</v>
       </c>
@@ -298,9 +292,6 @@
       <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="0" t="n">
-        <v>3</v>
-      </c>
       <c r="G4" s="0" t="n">
         <v>7054</v>
       </c>
@@ -330,9 +321,6 @@
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="0" t="n">
-        <v>4</v>
-      </c>
       <c r="G5" s="0" t="n">
         <v>6991</v>
       </c>
@@ -362,9 +350,6 @@
       <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="0" t="n">
-        <v>5</v>
-      </c>
       <c r="G6" s="0" t="n">
         <v>6893</v>
       </c>
@@ -394,9 +379,6 @@
       <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="0" t="n">
-        <v>6</v>
-      </c>
       <c r="G7" s="0" t="n">
         <v>6863</v>
       </c>
@@ -426,9 +408,6 @@
       <c r="E8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="0" t="n">
-        <v>7</v>
-      </c>
       <c r="G8" s="0" t="n">
         <v>7052</v>
       </c>
@@ -457,9 +436,6 @@
       </c>
       <c r="E9" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>8</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>7135</v>

</xml_diff>